<commit_message>
added results for cca
</commit_message>
<xml_diff>
--- a/Code/eval/results.xlsx
+++ b/Code/eval/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>RNN+LDA</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Unique words</t>
   </si>
   <si>
-    <t>glstm + CCA</t>
-  </si>
-  <si>
     <t>pp</t>
   </si>
   <si>
@@ -71,18 +68,9 @@
     <t>glstm + LDA 80</t>
   </si>
   <si>
-    <t>volledig</t>
-  </si>
-  <si>
-    <t>enkel bleu</t>
-  </si>
-  <si>
     <t>Google NIC (lstm)</t>
   </si>
   <si>
-    <t>Attention</t>
-  </si>
-  <si>
     <t>Jia guide + length normalization(gaussian)</t>
   </si>
   <si>
@@ -122,26 +110,119 @@
     <t>rnn_gauss_struct.json</t>
   </si>
   <si>
-    <t>rnnlda_struct.json</t>
-  </si>
-  <si>
     <t>glstm+lda 80+gauss</t>
   </si>
   <si>
-    <t>glstm + LDA</t>
-  </si>
-  <si>
-    <t>glstm_lda_80_25.52_struct.json</t>
-  </si>
-  <si>
     <t>glstm+lda+80</t>
+  </si>
+  <si>
+    <t>Attention+SF(lda 80)</t>
+  </si>
+  <si>
+    <t>Attention Xu</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>glstm + LDA120</t>
+  </si>
+  <si>
+    <t>glstm_lda_80_25.17_struct.json</t>
+  </si>
+  <si>
+    <t>glstm cca 128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beste model voor </t>
+  </si>
+  <si>
+    <t>model_checkpoint_flickr30k_paris_baseline_28.56.p</t>
+  </si>
+  <si>
+    <t>19.7</t>
+  </si>
+  <si>
+    <t>RNN+LDA 120</t>
+  </si>
+  <si>
+    <t>Beste Model volgens Bleu4 op validation</t>
+  </si>
+  <si>
+    <t>rnnlda_120_28.56</t>
+  </si>
+  <si>
+    <t>veel lengte 2!</t>
+  </si>
+  <si>
+    <t>rnnlda_120_gauss_28.56</t>
+  </si>
+  <si>
+    <t>glstm+cca+128</t>
+  </si>
+  <si>
+    <t>model_checkpoint_flickr30k_paris_baseline_24.82.p</t>
+  </si>
+  <si>
+    <t>glstm_cca_128_24.82</t>
+  </si>
+  <si>
+    <t>glstm_cca_128_24.82_struct.json</t>
+  </si>
+  <si>
+    <t>glstm cca 128+gauss</t>
+  </si>
+  <si>
+    <t>Rood zijn onze best performende :)</t>
+  </si>
+  <si>
+    <t>glstm cca 128+minhinge</t>
+  </si>
+  <si>
+    <t>glstm cca 256</t>
+  </si>
+  <si>
+    <t>glstm cca 256+gauss</t>
+  </si>
+  <si>
+    <t>glstm cca 256+hinge</t>
+  </si>
+  <si>
+    <t>Perturbed</t>
+  </si>
+  <si>
+    <t>glstm_cca_minhinge_128_24.82_struct.json</t>
+  </si>
+  <si>
+    <t>model_checkpoint_flickr30k_paris_baseline_23.62.p</t>
+  </si>
+  <si>
+    <t>glstm+cca+256</t>
+  </si>
+  <si>
+    <t>24&lt;= lengte 4</t>
+  </si>
+  <si>
+    <t>glstm_cca_256_gauss_23.62_struct.json</t>
+  </si>
+  <si>
+    <t>glstm_cca_256_23.62_struct.json</t>
+  </si>
+  <si>
+    <t>alles groter dan 7</t>
+  </si>
+  <si>
+    <t>glstm_cca_256_minhinge_23.62_struct.json</t>
+  </si>
+  <si>
+    <t>Kijken naar implementatie -&gt; lijkt geen effect te hebben op zinlengte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +242,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,13 +274,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -507,36 +596,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="B1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -562,13 +651,13 @@
       <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
+      <c r="P2" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -598,50 +687,48 @@
         <v>7.1360000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>32</v>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>30</v>
-      </c>
-      <c r="E4">
-        <v>66</v>
-      </c>
-      <c r="F4">
-        <v>44.6</v>
-      </c>
-      <c r="G4">
-        <v>29.2</v>
-      </c>
-      <c r="H4">
-        <v>18.7</v>
-      </c>
-      <c r="J4">
-        <v>14.8</v>
+        <v>28.56</v>
+      </c>
+      <c r="E4" s="4">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="F4" s="4">
+        <v>44</v>
+      </c>
+      <c r="G4" s="4">
+        <v>29.1</v>
+      </c>
+      <c r="H4" s="4">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4">
+        <v>14.38</v>
       </c>
       <c r="K4">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="L4">
-        <v>7.5970000000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
+        <v>7.5890000000000004</v>
+      </c>
+      <c r="M4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>20.059999999999999</v>
@@ -671,36 +758,33 @@
         <v>7.891</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6">
-        <v>270</v>
-      </c>
-      <c r="L6">
-        <v>9.8450000000000006</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>51.6</v>
+      </c>
+      <c r="F6">
+        <v>31.3</v>
+      </c>
+      <c r="G6">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="H6">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>28.33</v>
@@ -721,12 +805,12 @@
         <v>14.66</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>25.52</v>
@@ -735,41 +819,45 @@
         <v>61.4</v>
       </c>
       <c r="F9">
-        <v>40.299999999999997</v>
+        <v>40.4</v>
       </c>
       <c r="G9">
-        <v>25.9</v>
+        <v>26</v>
       </c>
       <c r="H9">
         <v>16.7</v>
       </c>
       <c r="J9">
-        <v>14.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
+        <v>14.7</v>
+      </c>
+      <c r="K9">
+        <v>335</v>
+      </c>
+      <c r="L9">
+        <v>8.3279999999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10">
+        <v>18</v>
+      </c>
+      <c r="E10" s="4">
         <v>61.2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="4">
         <v>41.1</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <v>27.3</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4">
         <v>18.2</v>
       </c>
-      <c r="J10">
+      <c r="I10" s="4"/>
+      <c r="J10" s="4">
         <v>16.920000000000002</v>
       </c>
       <c r="K10">
@@ -779,18 +867,15 @@
         <v>10.356999999999999</v>
       </c>
       <c r="M10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E11">
         <v>62.4</v>
@@ -814,147 +899,408 @@
         <v>10.141999999999999</v>
       </c>
       <c r="M11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>28.56</v>
+      </c>
+      <c r="E12" s="4">
+        <v>62.7</v>
+      </c>
+      <c r="F12" s="4">
+        <v>42.6</v>
+      </c>
+      <c r="G12" s="4">
+        <v>28.8</v>
+      </c>
+      <c r="H12" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4">
+        <v>16.62</v>
+      </c>
+      <c r="K12">
+        <v>192</v>
+      </c>
+      <c r="L12">
+        <v>10.329000000000001</v>
+      </c>
+      <c r="M12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13">
+        <v>59.8</v>
+      </c>
+      <c r="F13">
+        <v>39.1</v>
+      </c>
+      <c r="G13">
+        <v>25.1</v>
+      </c>
+      <c r="H13">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14">
+        <v>63.5</v>
+      </c>
+      <c r="F14">
+        <v>42.5</v>
+      </c>
+      <c r="G14">
+        <v>27.9</v>
+      </c>
+      <c r="H14">
+        <v>18</v>
+      </c>
+      <c r="J14">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15">
+        <v>62.1</v>
+      </c>
+      <c r="F15">
+        <v>41.6</v>
+      </c>
+      <c r="G15">
+        <v>27.6</v>
+      </c>
+      <c r="H15">
+        <v>18.2</v>
+      </c>
+      <c r="J15">
+        <v>16.77</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>63.5</v>
+      </c>
+      <c r="F16">
+        <v>42.4</v>
+      </c>
+      <c r="G16">
+        <v>27.9</v>
+      </c>
+      <c r="H16">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="J16">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="4">
+        <v>63.7</v>
+      </c>
+      <c r="F17" s="4">
+        <v>43.4</v>
+      </c>
+      <c r="G17" s="4">
+        <v>29.2</v>
+      </c>
+      <c r="H17" s="4">
+        <v>19.3</v>
+      </c>
+      <c r="J17">
+        <v>15.76</v>
+      </c>
+      <c r="K17">
+        <v>347</v>
+      </c>
+      <c r="L17">
+        <v>7.96</v>
+      </c>
+      <c r="M17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18">
+        <v>62.1</v>
+      </c>
+      <c r="F18">
+        <v>41.9</v>
+      </c>
+      <c r="G18">
+        <v>28.2</v>
+      </c>
+      <c r="H18">
+        <v>18.7</v>
+      </c>
+      <c r="J18" s="4">
+        <v>17.18</v>
+      </c>
+      <c r="K18">
+        <v>383</v>
+      </c>
+      <c r="L18">
+        <v>10.362</v>
+      </c>
+      <c r="M18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19">
+        <v>63.8</v>
+      </c>
+      <c r="F19">
+        <v>43.4</v>
+      </c>
+      <c r="G19">
+        <v>29.2</v>
+      </c>
+      <c r="H19">
+        <v>19.3</v>
+      </c>
+      <c r="J19">
+        <v>15.69</v>
+      </c>
+      <c r="K19">
+        <v>346</v>
+      </c>
+      <c r="L19">
+        <v>7.94</v>
+      </c>
+      <c r="M19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21">
+        <v>66.3</v>
+      </c>
+      <c r="F21">
+        <v>42.3</v>
+      </c>
+      <c r="G21">
+        <v>27.7</v>
+      </c>
+      <c r="H21">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="F22">
+        <v>44.6</v>
+      </c>
+      <c r="G22">
+        <v>30.5</v>
+      </c>
+      <c r="H22">
+        <v>20.6</v>
+      </c>
+      <c r="J22">
+        <v>17.91</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23">
+        <v>59.8</v>
+      </c>
+      <c r="F23">
+        <v>41.3</v>
+      </c>
+      <c r="G23">
+        <v>29.3</v>
+      </c>
+      <c r="H23">
+        <v>19.2</v>
+      </c>
+      <c r="J23">
+        <v>18.579999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="F24">
+        <v>43.9</v>
+      </c>
+      <c r="G24">
+        <v>29.6</v>
+      </c>
+      <c r="H24">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="J24">
+        <v>18.46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25">
+        <v>57.3</v>
+      </c>
+      <c r="F25">
+        <v>36.9</v>
+      </c>
+      <c r="G25">
         <v>24</v>
       </c>
-      <c r="D12">
-        <v>27.65</v>
-      </c>
-      <c r="E12">
-        <v>61</v>
-      </c>
-      <c r="F12">
-        <v>41.3</v>
-      </c>
-      <c r="G12">
-        <v>27.6</v>
-      </c>
-      <c r="H12">
-        <v>18.399999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="H25">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26">
+        <v>67</v>
+      </c>
+      <c r="F26">
+        <v>47.5</v>
+      </c>
+      <c r="G26">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15">
-        <v>66.3</v>
-      </c>
-      <c r="F15">
-        <v>42.3</v>
-      </c>
-      <c r="G15">
-        <v>27.7</v>
-      </c>
-      <c r="H15">
-        <v>18.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16">
-        <v>64.599999999999994</v>
-      </c>
-      <c r="F16">
-        <v>44.6</v>
-      </c>
-      <c r="G16">
-        <v>30.5</v>
-      </c>
-      <c r="H16">
-        <v>20.6</v>
-      </c>
-      <c r="J16">
-        <v>17.91</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17">
-        <v>59.8</v>
-      </c>
-      <c r="F17">
-        <v>41.3</v>
-      </c>
-      <c r="G17">
-        <v>29.3</v>
-      </c>
-      <c r="H17">
-        <v>19.2</v>
-      </c>
-      <c r="J17">
-        <v>18.579999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18">
-        <v>66.900000000000006</v>
-      </c>
-      <c r="F18">
-        <v>43.9</v>
-      </c>
-      <c r="G18">
-        <v>29.6</v>
-      </c>
-      <c r="H18">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="J18">
-        <v>18.46</v>
-      </c>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19">
-        <v>57.3</v>
-      </c>
-      <c r="F19">
-        <v>36.9</v>
-      </c>
-      <c r="G19">
-        <v>24</v>
-      </c>
-      <c r="H19">
-        <v>15.7</v>
+      <c r="H26">
+        <v>24.3</v>
+      </c>
+      <c r="J26">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
+      <c r="K34">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+      <c r="K35">
+        <v>19.8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:E19">
-    <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
+  <conditionalFormatting sqref="J3:J26">
+    <cfRule type="top10" dxfId="4" priority="14" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F19">
-    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
+  <conditionalFormatting sqref="L14 E3:E27">
+    <cfRule type="top10" dxfId="3" priority="15" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G19">
-    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
+  <conditionalFormatting sqref="F3:F27">
+    <cfRule type="top10" dxfId="2" priority="19" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H19">
-    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
+  <conditionalFormatting sqref="G3:G27">
+    <cfRule type="top10" dxfId="1" priority="22" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J19">
-    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+  <conditionalFormatting sqref="H3:H27">
+    <cfRule type="top10" dxfId="0" priority="25" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
pert cca > lda 80
</commit_message>
<xml_diff>
--- a/Code/eval/results.xlsx
+++ b/Code/eval/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>RNN+LDA</t>
   </si>
@@ -272,13 +272,10 @@
     <t>glstm_cca_512</t>
   </si>
   <si>
-    <t>glstm pert cca</t>
-  </si>
-  <si>
-    <t>29,27 (15B4)</t>
-  </si>
-  <si>
-    <t>gmstm lda 120</t>
+    <t>glstm_pert_cca128_struct.json</t>
+  </si>
+  <si>
+    <t>glstm + cca 128 pert</t>
   </si>
 </sst>
 </file>
@@ -760,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +766,7 @@
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
@@ -1654,13 +1651,28 @@
       <c r="B33" t="s">
         <v>82</v>
       </c>
-      <c r="D33" t="s">
+      <c r="C33" t="s">
         <v>83</v>
+      </c>
+      <c r="D33">
+        <v>29.27</v>
+      </c>
+      <c r="E33">
+        <v>57.4</v>
+      </c>
+      <c r="F33">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="G33">
+        <v>22.6</v>
+      </c>
+      <c r="H33">
+        <v>14.3</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
blijkbaar nog dingen veranderd :D
</commit_message>
<xml_diff>
--- a/Code/eval/results.xlsx
+++ b/Code/eval/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="84">
   <si>
     <t>RNN+LDA</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Karpathy</t>
   </si>
   <si>
-    <t>BP</t>
-  </si>
-  <si>
     <t>Avg sentence length</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>LSTM</t>
   </si>
   <si>
-    <t>glstm + LDA 80</t>
-  </si>
-  <si>
     <t>Google NIC (lstm)</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>lstm_20.06_struct.json</t>
   </si>
   <si>
-    <t>glstm_lda80_28.33_struct.json</t>
-  </si>
-  <si>
     <t>lstm_20.06_gauss_struct.json</t>
   </si>
   <si>
@@ -173,9 +164,6 @@
     <t>glstm cca 256+gauss</t>
   </si>
   <si>
-    <t>glstm cca 256+hinge</t>
-  </si>
-  <si>
     <t>Perturbed</t>
   </si>
   <si>
@@ -200,9 +188,6 @@
     <t>alles groter dan 7</t>
   </si>
   <si>
-    <t>glstm_cca_256_minhinge_23.62_struct.json</t>
-  </si>
-  <si>
     <t>glstm lda</t>
   </si>
   <si>
@@ -248,9 +233,6 @@
     <t>GLSTM+LDA80+pert</t>
   </si>
   <si>
-    <t>GLSTM+LDA80+pert+gauss</t>
-  </si>
-  <si>
     <t>Beam effect</t>
   </si>
   <si>
@@ -276,6 +258,24 @@
   </si>
   <si>
     <t>glstm + cca 128 pert</t>
+  </si>
+  <si>
+    <t>* Not in train = niet in ongewijzigde train</t>
+  </si>
+  <si>
+    <t>glstm cca 256 pert</t>
+  </si>
+  <si>
+    <t>glstm lda 120 pert</t>
+  </si>
+  <si>
+    <t>met brevity penalty</t>
+  </si>
+  <si>
+    <t>glstm lda pert 120</t>
+  </si>
+  <si>
+    <t>model_checkpoint_flickr30k_paris_baseline_29.75.p</t>
   </si>
 </sst>
 </file>
@@ -348,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -361,11 +361,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <u/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -392,6 +413,41 @@
     </dxf>
     <dxf>
       <font>
+        <u/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
       </font>
@@ -416,41 +472,6 @@
     </dxf>
     <dxf>
       <font>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
       </font>
@@ -471,6 +492,41 @@
       <font>
         <b/>
         <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
       </font>
     </dxf>
     <dxf>
@@ -755,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q62"/>
+  <dimension ref="B1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,26 +823,27 @@
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" customWidth="1"/>
-    <col min="15" max="15" width="35.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" customWidth="1"/>
+    <col min="14" max="14" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -800,31 +857,28 @@
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -844,219 +898,232 @@
       <c r="H3">
         <v>17.8</v>
       </c>
+      <c r="I3">
+        <v>14.29</v>
+      </c>
       <c r="J3">
-        <v>14.29</v>
+        <v>233</v>
       </c>
       <c r="K3">
-        <v>233</v>
+        <v>7.1360000000000001</v>
       </c>
       <c r="L3">
-        <v>7.1360000000000001</v>
+        <v>785</v>
       </c>
       <c r="M3">
-        <v>785</v>
-      </c>
-      <c r="N3">
         <v>392</v>
       </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4">
+        <v>0.85</v>
+      </c>
+      <c r="E4" s="8">
+        <f>E3*$D$4</f>
+        <v>55.165000000000006</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" ref="F4:H4" si="0">F3*$D$4</f>
+        <v>36.634999999999998</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>23.885000000000002</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>15.13</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>28.56</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E5" s="4">
         <v>65.400000000000006</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F5" s="4">
         <v>44</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G5" s="4">
         <v>29.1</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H5" s="4">
         <v>19</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4">
+      <c r="I5" s="4">
         <v>14.38</v>
       </c>
-      <c r="K4">
+      <c r="J5">
         <v>189</v>
       </c>
-      <c r="L4">
+      <c r="K5">
         <v>7.5890000000000004</v>
       </c>
-      <c r="M4">
+      <c r="L5">
         <v>823</v>
       </c>
-      <c r="N4">
+      <c r="M5">
         <v>387</v>
       </c>
-      <c r="O4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
+      <c r="N5" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
         <v>20.059999999999999</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>62.1</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>41.4</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>27.1</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <v>17.600000000000001</v>
       </c>
-      <c r="I5">
-        <v>0.90300000000000002</v>
-      </c>
-      <c r="J5">
+      <c r="I6">
         <v>15.08</v>
       </c>
-      <c r="K5">
+      <c r="J6">
         <v>327</v>
       </c>
-      <c r="L5">
+      <c r="K6">
         <v>7.891</v>
       </c>
-      <c r="M5">
+      <c r="L6">
         <v>723</v>
       </c>
-      <c r="N5">
+      <c r="M6">
         <v>399</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6">
-        <v>23.16</v>
-      </c>
-      <c r="E6">
-        <v>64.400000000000006</v>
-      </c>
-      <c r="F6">
-        <v>43.2</v>
-      </c>
-      <c r="G6">
-        <v>28.1</v>
-      </c>
-      <c r="H6">
-        <v>17.8</v>
-      </c>
-      <c r="J6">
-        <v>15.95</v>
-      </c>
-      <c r="K6">
-        <v>296</v>
-      </c>
-      <c r="L6">
-        <v>8.3249999999999993</v>
-      </c>
-      <c r="M6">
-        <v>775</v>
-      </c>
-      <c r="N6" s="5">
-        <v>490</v>
-      </c>
       <c r="O6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>23.16</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="F7">
+        <v>43.2</v>
+      </c>
+      <c r="G7">
+        <v>28.1</v>
+      </c>
+      <c r="H7">
+        <v>17.8</v>
+      </c>
+      <c r="I7">
+        <v>15.95</v>
+      </c>
+      <c r="J7">
+        <v>296</v>
+      </c>
+      <c r="K7">
+        <v>8.3249999999999993</v>
+      </c>
+      <c r="L7">
+        <v>775</v>
+      </c>
+      <c r="M7" s="5">
+        <v>490</v>
+      </c>
+      <c r="N7" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8">
+        <v>23.16</v>
+      </c>
+      <c r="E8" s="4">
         <v>62.7</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F8" s="4">
         <v>42.5</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G8" s="4">
         <v>28.8</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H8" s="4">
         <v>19.399999999999999</v>
       </c>
-      <c r="J7" s="4">
+      <c r="I8" s="4">
         <v>17.399999999999999</v>
       </c>
-      <c r="K7">
+      <c r="J8">
         <v>323</v>
       </c>
-      <c r="L7">
+      <c r="K8">
         <v>10.432</v>
       </c>
-      <c r="M7" s="4">
+      <c r="L8" s="4">
         <v>907</v>
       </c>
-      <c r="N7" s="4">
+      <c r="M8" s="4">
         <v>541</v>
       </c>
-      <c r="O7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>28.33</v>
-      </c>
-      <c r="E8">
-        <v>61.8</v>
-      </c>
-      <c r="F8">
-        <v>40.700000000000003</v>
-      </c>
-      <c r="G8">
-        <v>26.6</v>
-      </c>
-      <c r="H8">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="J8">
-        <v>14.66</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>25.52</v>
@@ -1073,22 +1140,25 @@
       <c r="H9">
         <v>16.7</v>
       </c>
+      <c r="I9">
+        <v>14.7</v>
+      </c>
       <c r="J9">
-        <v>14.7</v>
+        <v>335</v>
       </c>
       <c r="K9">
-        <v>335</v>
-      </c>
-      <c r="L9">
         <v>8.3279999999999994</v>
       </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>20.059999999999999</v>
@@ -1105,32 +1175,34 @@
       <c r="H10" s="4">
         <v>18.2</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4">
+      <c r="I10" s="4">
         <v>16.920000000000002</v>
       </c>
+      <c r="J10">
+        <v>351</v>
+      </c>
       <c r="K10">
-        <v>351</v>
-      </c>
-      <c r="L10">
         <v>10.356999999999999</v>
       </c>
-      <c r="M10" s="4">
+      <c r="L10" s="4">
         <v>905</v>
       </c>
-      <c r="N10">
+      <c r="M10">
         <v>437</v>
       </c>
+      <c r="N10" t="s">
+        <v>14</v>
+      </c>
       <c r="O10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
       </c>
       <c r="D11">
         <v>26.29</v>
@@ -1147,31 +1219,34 @@
       <c r="H11">
         <v>18.600000000000001</v>
       </c>
+      <c r="I11">
+        <v>16.57</v>
+      </c>
       <c r="J11">
-        <v>16.57</v>
+        <v>239</v>
       </c>
       <c r="K11">
-        <v>239</v>
-      </c>
-      <c r="L11">
         <v>10.141999999999999</v>
       </c>
-      <c r="M11" s="4">
+      <c r="L11" s="4">
         <v>931</v>
       </c>
-      <c r="N11">
+      <c r="M11">
         <v>439</v>
       </c>
+      <c r="N11" t="s">
+        <v>18</v>
+      </c>
       <c r="O11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12">
         <v>28.56</v>
@@ -1188,29 +1263,31 @@
       <c r="H12" s="4">
         <v>19.5</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4">
+      <c r="I12" s="4">
         <v>16.62</v>
       </c>
+      <c r="J12">
+        <v>192</v>
+      </c>
       <c r="K12">
-        <v>192</v>
-      </c>
-      <c r="L12">
         <v>10.329000000000001</v>
       </c>
-      <c r="M12" s="4">
+      <c r="L12" s="4">
         <v>930</v>
       </c>
-      <c r="N12">
+      <c r="M12">
         <v>384</v>
       </c>
+      <c r="N12" t="s">
+        <v>18</v>
+      </c>
       <c r="O12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E13">
         <v>59.8</v>
@@ -1224,13 +1301,16 @@
       <c r="H13">
         <v>16.100000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D14">
         <v>24.82</v>
@@ -1247,28 +1327,31 @@
       <c r="H14">
         <v>18</v>
       </c>
+      <c r="I14">
+        <v>15.5</v>
+      </c>
       <c r="J14">
-        <v>15.5</v>
+        <v>276</v>
       </c>
       <c r="K14">
-        <v>276</v>
+        <v>7.9930000000000003</v>
       </c>
       <c r="L14">
-        <v>7.9930000000000003</v>
+        <v>786</v>
       </c>
       <c r="M14">
-        <v>786</v>
-      </c>
-      <c r="N14">
         <v>461</v>
       </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D15">
         <v>24.82</v>
@@ -1285,28 +1368,31 @@
       <c r="H15">
         <v>18.2</v>
       </c>
+      <c r="I15">
+        <v>16.77</v>
+      </c>
       <c r="J15">
-        <v>16.77</v>
+        <v>286</v>
       </c>
       <c r="K15">
-        <v>286</v>
-      </c>
-      <c r="L15">
         <v>10.382999999999999</v>
       </c>
-      <c r="M15" s="4">
+      <c r="L15" s="4">
         <v>911</v>
       </c>
-      <c r="N15">
+      <c r="M15">
         <v>482</v>
       </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>24.82</v>
@@ -1323,22 +1409,25 @@
       <c r="H16">
         <v>17.600000000000001</v>
       </c>
+      <c r="I16">
+        <v>15.5</v>
+      </c>
       <c r="J16">
-        <v>15.5</v>
+        <v>277</v>
       </c>
       <c r="K16">
-        <v>277</v>
-      </c>
-      <c r="L16">
         <v>7.9770000000000003</v>
+      </c>
+      <c r="O16" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D17">
         <v>23.62</v>
@@ -1355,31 +1444,34 @@
       <c r="H17" s="4">
         <v>19.3</v>
       </c>
+      <c r="I17">
+        <v>15.76</v>
+      </c>
       <c r="J17">
-        <v>15.76</v>
+        <v>347</v>
       </c>
       <c r="K17">
-        <v>347</v>
+        <v>7.96</v>
       </c>
       <c r="L17">
-        <v>7.96</v>
-      </c>
-      <c r="M17">
         <v>775</v>
       </c>
-      <c r="N17" s="4">
+      <c r="M17" s="4">
         <v>557</v>
       </c>
+      <c r="N17" t="s">
+        <v>50</v>
+      </c>
       <c r="O17" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D18">
         <v>23.62</v>
@@ -1396,42 +1488,34 @@
       <c r="H18">
         <v>18.7</v>
       </c>
+      <c r="I18" s="4">
+        <v>17.18</v>
+      </c>
       <c r="J18" s="4">
-        <v>17.18</v>
-      </c>
-      <c r="K18" s="4">
         <v>383</v>
       </c>
-      <c r="L18">
+      <c r="K18">
         <v>10.362</v>
       </c>
+      <c r="L18" s="4">
+        <v>915</v>
+      </c>
       <c r="M18" s="4">
-        <v>915</v>
-      </c>
-      <c r="N18" s="4">
         <v>602</v>
       </c>
+      <c r="N18" t="s">
+        <v>53</v>
+      </c>
       <c r="O18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19">
-        <v>23.62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E20">
         <v>63.3</v>
@@ -1445,13 +1529,31 @@
       <c r="H20">
         <v>18.3</v>
       </c>
+      <c r="I20">
+        <v>15.08</v>
+      </c>
+      <c r="J20">
+        <v>308</v>
+      </c>
+      <c r="K20">
+        <v>7.81</v>
+      </c>
+      <c r="L20">
+        <v>833</v>
+      </c>
+      <c r="M20">
+        <v>531</v>
+      </c>
+      <c r="O20" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E21">
         <v>40.700000000000003</v>
@@ -1465,29 +1567,32 @@
       <c r="H21">
         <v>7.6</v>
       </c>
+      <c r="I21">
+        <v>12.82</v>
+      </c>
       <c r="J21">
-        <v>12.82</v>
+        <v>721</v>
       </c>
       <c r="K21">
-        <v>721</v>
-      </c>
-      <c r="L21">
         <v>10.542999999999999</v>
       </c>
+      <c r="L21" s="6">
+        <v>991</v>
+      </c>
       <c r="M21" s="6">
-        <v>991</v>
-      </c>
-      <c r="N21" s="6">
         <v>927</v>
       </c>
-    </row>
-    <row r="22" spans="2:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="O21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E23">
         <v>66.3</v>
@@ -1501,10 +1606,13 @@
       <c r="H23">
         <v>18.3</v>
       </c>
+      <c r="O23" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E24">
         <v>64.599999999999994</v>
@@ -1518,13 +1626,16 @@
       <c r="H24">
         <v>20.6</v>
       </c>
-      <c r="J24">
+      <c r="I24">
         <v>17.91</v>
+      </c>
+      <c r="O24" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E25">
         <v>59.8</v>
@@ -1538,13 +1649,16 @@
       <c r="H25">
         <v>19.2</v>
       </c>
-      <c r="J25">
+      <c r="I25">
         <v>18.579999999999998</v>
+      </c>
+      <c r="O25" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E26">
         <v>66.900000000000006</v>
@@ -1558,8 +1672,11 @@
       <c r="H26">
         <v>19.899999999999999</v>
       </c>
-      <c r="J26">
+      <c r="I26">
         <v>18.46</v>
+      </c>
+      <c r="O26" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
@@ -1578,10 +1695,13 @@
       <c r="H27">
         <v>15.7</v>
       </c>
+      <c r="O27" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E28">
         <v>67</v>
@@ -1595,21 +1715,24 @@
       <c r="H28">
         <v>24.3</v>
       </c>
-      <c r="J28">
+      <c r="I28">
         <v>19.399999999999999</v>
+      </c>
+      <c r="O28" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D31">
         <v>29.7</v>
@@ -1626,33 +1749,45 @@
       <c r="H31">
         <v>9</v>
       </c>
+      <c r="I31">
+        <v>12.52</v>
+      </c>
       <c r="J31">
-        <v>12.52</v>
+        <v>248</v>
       </c>
       <c r="K31">
-        <v>248</v>
+        <v>13.862</v>
       </c>
       <c r="L31">
-        <v>13.862</v>
+        <v>993</v>
       </c>
       <c r="M31">
-        <v>993</v>
-      </c>
-      <c r="N31">
         <v>738</v>
+      </c>
+      <c r="N31" t="s">
+        <v>78</v>
+      </c>
+      <c r="O31" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="D32">
+        <v>29.75</v>
+      </c>
+      <c r="O32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D33">
         <v>29.27</v>
@@ -1669,92 +1804,127 @@
       <c r="H33">
         <v>14.3</v>
       </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>13.53</v>
+      </c>
+      <c r="J33">
+        <v>179</v>
+      </c>
+      <c r="K33">
+        <v>8.9540000000000006</v>
+      </c>
+      <c r="L33">
+        <v>844</v>
+      </c>
+      <c r="M33">
+        <v>420</v>
+      </c>
+      <c r="N33" t="s">
+        <v>78</v>
+      </c>
+      <c r="O33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+      <c r="O34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J38">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" t="s">
-        <v>36</v>
-      </c>
-      <c r="K38">
-        <v>19.7</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>41</v>
-      </c>
       <c r="D39" t="s">
-        <v>42</v>
-      </c>
-      <c r="K39">
+        <v>39</v>
+      </c>
+      <c r="J39">
         <v>19.8</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D40" t="s">
-        <v>52</v>
-      </c>
-      <c r="K40">
+        <v>48</v>
+      </c>
+      <c r="J40">
         <v>19.8</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D41" t="s">
-        <v>66</v>
-      </c>
-      <c r="K41">
+        <v>61</v>
+      </c>
+      <c r="J41">
         <v>20.2</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D42" t="s">
-        <v>78</v>
-      </c>
-      <c r="K42">
+        <v>72</v>
+      </c>
+      <c r="J42">
         <v>19.8</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" t="s">
+        <v>83</v>
+      </c>
+      <c r="J43">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D46" s="3">
         <v>23.16</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>1</v>
       </c>
@@ -1771,7 +1941,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>5</v>
       </c>
@@ -1788,12 +1958,24 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>63.6</v>
+      </c>
+      <c r="F49">
+        <v>42.9</v>
+      </c>
+      <c r="G49">
+        <v>28.4</v>
+      </c>
+      <c r="H49">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>25</v>
       </c>
@@ -1810,7 +1992,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>50</v>
       </c>
@@ -1826,23 +2008,23 @@
       <c r="H51">
         <v>17.8</v>
       </c>
+      <c r="I51">
+        <v>15.95</v>
+      </c>
       <c r="J51">
-        <v>15.95</v>
+        <v>296</v>
       </c>
       <c r="K51">
-        <v>296</v>
+        <v>8.3249999999999993</v>
       </c>
       <c r="L51">
-        <v>8.3249999999999993</v>
+        <v>775</v>
       </c>
       <c r="M51">
-        <v>775</v>
-      </c>
-      <c r="N51">
         <v>490</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>75</v>
       </c>
@@ -1859,7 +2041,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>100</v>
       </c>
@@ -1876,15 +2058,15 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D55" s="3">
         <v>23.16</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>1</v>
       </c>
@@ -1901,7 +2083,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>5</v>
       </c>
@@ -1918,7 +2100,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>10</v>
       </c>
@@ -1935,29 +2117,41 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>25</v>
       </c>
-    </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>62.9</v>
+      </c>
+      <c r="F59">
+        <v>42.7</v>
+      </c>
+      <c r="G59">
+        <v>28.9</v>
+      </c>
+      <c r="H59">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>50</v>
       </c>
       <c r="E60">
-        <v>65.400000000000006</v>
+        <v>62.7</v>
       </c>
       <c r="F60">
-        <v>44</v>
+        <v>42.5</v>
       </c>
       <c r="G60">
-        <v>29.1</v>
+        <v>28.8</v>
       </c>
       <c r="H60">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>75</v>
       </c>
@@ -1974,7 +2168,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>100</v>
       </c>
@@ -1983,65 +2177,65 @@
   <mergeCells count="1">
     <mergeCell ref="E1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="J3:J28">
-    <cfRule type="top10" dxfId="19" priority="29" rank="1"/>
+  <conditionalFormatting sqref="K14:K16 E3:E29 E31 F4:H4">
+    <cfRule type="top10" dxfId="27" priority="30" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E29 L14:L16 E31">
-    <cfRule type="top10" dxfId="18" priority="30" rank="1"/>
+  <conditionalFormatting sqref="F31 F3 F5:F29">
+    <cfRule type="top10" dxfId="26" priority="34" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F29 F31">
-    <cfRule type="top10" dxfId="17" priority="34" rank="1"/>
+  <conditionalFormatting sqref="G31 G3 G5:G29">
+    <cfRule type="top10" dxfId="25" priority="37" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G29 G31">
-    <cfRule type="top10" dxfId="16" priority="37" rank="1"/>
+  <conditionalFormatting sqref="H31 H3 H5:H29">
+    <cfRule type="top10" dxfId="24" priority="40" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H29 H31">
-    <cfRule type="top10" dxfId="15" priority="40" rank="1"/>
+  <conditionalFormatting sqref="E47:E53">
+    <cfRule type="top10" dxfId="23" priority="8" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E21">
-    <cfRule type="top10" dxfId="14" priority="15" rank="1"/>
+  <conditionalFormatting sqref="F47:F53">
+    <cfRule type="top10" dxfId="22" priority="7" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F21">
-    <cfRule type="top10" dxfId="13" priority="14" rank="1"/>
+  <conditionalFormatting sqref="G47:G53">
+    <cfRule type="top10" dxfId="21" priority="6" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G21">
-    <cfRule type="top10" dxfId="12" priority="13" rank="1"/>
+  <conditionalFormatting sqref="H47:H53">
+    <cfRule type="top10" dxfId="20" priority="5" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H21">
-    <cfRule type="top10" dxfId="11" priority="12" rank="1"/>
+  <conditionalFormatting sqref="E56:E62">
+    <cfRule type="top10" dxfId="19" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F56:F62">
+    <cfRule type="top10" dxfId="18" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G56:G62">
+    <cfRule type="top10" dxfId="17" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H56:H62">
+    <cfRule type="top10" dxfId="16" priority="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I28">
+    <cfRule type="top10" dxfId="15" priority="41" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E21 F4:H4">
+    <cfRule type="top10" dxfId="14" priority="52" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3 F5:F21">
+    <cfRule type="top10" dxfId="13" priority="54" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3 G5:G21">
+    <cfRule type="top10" dxfId="12" priority="56" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3 H5:H21">
+    <cfRule type="top10" dxfId="11" priority="58" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I21">
+    <cfRule type="top10" dxfId="10" priority="60" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J21">
-    <cfRule type="top10" dxfId="10" priority="11" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="62" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K21">
-    <cfRule type="top10" dxfId="9" priority="10" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L21">
-    <cfRule type="top10" dxfId="8" priority="9" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47:E53">
-    <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47:F53">
-    <cfRule type="top10" dxfId="6" priority="7" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G47:G53">
-    <cfRule type="top10" dxfId="5" priority="6" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H47:H53">
-    <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E56:E62">
-    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F56:F62">
-    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G56:G62">
-    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H56:H62">
-    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="64" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
results van frequentie + once + lda120pert
</commit_message>
<xml_diff>
--- a/Code/eval/results.xlsx
+++ b/Code/eval/results.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="197">
   <si>
     <t>RNN+LDA</t>
   </si>
@@ -276,6 +278,345 @@
   </si>
   <si>
     <t>model_checkpoint_flickr30k_paris_baseline_29.75.p</t>
+  </si>
+  <si>
+    <t>glstm lda 120 pert gauss</t>
+  </si>
+  <si>
+    <t>glstm_lda120_pert_struct.json</t>
+  </si>
+  <si>
+    <t>Heel veel hele grote zinnnen</t>
+  </si>
+  <si>
+    <t>glstm lda, img once</t>
+  </si>
+  <si>
+    <t>model_checkpoint_flickr30k_paris_baseline_24.58.p</t>
+  </si>
+  <si>
+    <t>Number of length 3sentences :4</t>
+  </si>
+  <si>
+    <t>Number of length 4sentences :12</t>
+  </si>
+  <si>
+    <t>Number of length 5sentences :22</t>
+  </si>
+  <si>
+    <t>Number of length 6sentences :139</t>
+  </si>
+  <si>
+    <t>Number of length 7sentences :200</t>
+  </si>
+  <si>
+    <t>Number of length 8sentences :114</t>
+  </si>
+  <si>
+    <t>Number of length 9sentences :235</t>
+  </si>
+  <si>
+    <t>Number of length 10sentences :150</t>
+  </si>
+  <si>
+    <t>Number of length 11sentences :101</t>
+  </si>
+  <si>
+    <t>Number of length 12sentences :18</t>
+  </si>
+  <si>
+    <t>Number of length 13sentences :3</t>
+  </si>
+  <si>
+    <t>Number of length 14sentences :2</t>
+  </si>
+  <si>
+    <t>gLSTM LDA</t>
+  </si>
+  <si>
+    <t>gLSTM LDA gauss</t>
+  </si>
+  <si>
+    <t>Number of length 7sentences :1</t>
+  </si>
+  <si>
+    <t>Number of length 8sentences :21</t>
+  </si>
+  <si>
+    <t>Number of length 9sentences :170</t>
+  </si>
+  <si>
+    <t>Number of length 10sentences :304</t>
+  </si>
+  <si>
+    <t>Number of length 11sentences :373</t>
+  </si>
+  <si>
+    <t>Number of length 12sentences :120</t>
+  </si>
+  <si>
+    <t>Number of length 13sentences :10</t>
+  </si>
+  <si>
+    <t>Number of length 14sentences :1</t>
+  </si>
+  <si>
+    <t>RNN</t>
+  </si>
+  <si>
+    <t>Number of length 2sentences :11</t>
+  </si>
+  <si>
+    <t>Number of length 3sentences :5</t>
+  </si>
+  <si>
+    <t>Number of length 4sentences :27</t>
+  </si>
+  <si>
+    <t>Number of length 5sentences :96</t>
+  </si>
+  <si>
+    <t>Number of length 6sentences :228</t>
+  </si>
+  <si>
+    <t>Number of length 7sentences :328</t>
+  </si>
+  <si>
+    <t>Number of length 8sentences :102</t>
+  </si>
+  <si>
+    <t>Number of length 9sentences :93</t>
+  </si>
+  <si>
+    <t>Number of length 10sentences :26</t>
+  </si>
+  <si>
+    <t>Number of length 11sentences :61</t>
+  </si>
+  <si>
+    <t>Number of length 12sentences :19</t>
+  </si>
+  <si>
+    <t>Number of length 13sentences :1</t>
+  </si>
+  <si>
+    <t>Number of length 15sentences :1</t>
+  </si>
+  <si>
+    <t>Number of length 20sentences :1</t>
+  </si>
+  <si>
+    <t>Number of length 7sentences :3</t>
+  </si>
+  <si>
+    <t>Number of length 8sentences :54</t>
+  </si>
+  <si>
+    <t>Number of length 9sentences :284</t>
+  </si>
+  <si>
+    <t>Number of length 10sentences :196</t>
+  </si>
+  <si>
+    <t>Number of length 11sentences :402</t>
+  </si>
+  <si>
+    <t>Number of length 12sentences :52</t>
+  </si>
+  <si>
+    <t>Number of length 13sentences :6</t>
+  </si>
+  <si>
+    <t>RNN Gauss</t>
+  </si>
+  <si>
+    <t>a 2217</t>
+  </si>
+  <si>
+    <t>in 836</t>
+  </si>
+  <si>
+    <t>is 685</t>
+  </si>
+  <si>
+    <t>of 486</t>
+  </si>
+  <si>
+    <t>man 471</t>
+  </si>
+  <si>
+    <t>shirt 417</t>
+  </si>
+  <si>
+    <t>a 2326</t>
+  </si>
+  <si>
+    <t>in 769</t>
+  </si>
+  <si>
+    <t>man 558</t>
+  </si>
+  <si>
+    <t>is 546</t>
+  </si>
+  <si>
+    <t>are 435</t>
+  </si>
+  <si>
+    <t>of 431</t>
+  </si>
+  <si>
+    <t>shirt 336</t>
+  </si>
+  <si>
+    <t>RNN LDA</t>
+  </si>
+  <si>
+    <t>umber of length 2sentences :9</t>
+  </si>
+  <si>
+    <t>Number of length 4sentences :15</t>
+  </si>
+  <si>
+    <t>Number of length 5sentences :76</t>
+  </si>
+  <si>
+    <t>Number of length 6sentences :200</t>
+  </si>
+  <si>
+    <t>Number of length 7sentences :308</t>
+  </si>
+  <si>
+    <t>Number of length 8sentences :91</t>
+  </si>
+  <si>
+    <t>Number of length 9sentences :101</t>
+  </si>
+  <si>
+    <t>Number of length 10sentences :56</t>
+  </si>
+  <si>
+    <t>Number of length 11sentences :125</t>
+  </si>
+  <si>
+    <t>Number of length 12sentences :12</t>
+  </si>
+  <si>
+    <t>a 1821</t>
+  </si>
+  <si>
+    <t>in 578</t>
+  </si>
+  <si>
+    <t>man 568</t>
+  </si>
+  <si>
+    <t>is 549</t>
+  </si>
+  <si>
+    <t>the 287</t>
+  </si>
+  <si>
+    <t>shirt 284</t>
+  </si>
+  <si>
+    <t>of 267</t>
+  </si>
+  <si>
+    <t>Number of length 3sentences :6</t>
+  </si>
+  <si>
+    <t>Number of length 4sentences :26</t>
+  </si>
+  <si>
+    <t>Number of length 5sentences :49</t>
+  </si>
+  <si>
+    <t>Number of length 6sentences :137</t>
+  </si>
+  <si>
+    <t>Number of length 7sentences :239</t>
+  </si>
+  <si>
+    <t>Number of length 8sentences :138</t>
+  </si>
+  <si>
+    <t>Number of length 9sentences :217</t>
+  </si>
+  <si>
+    <t>Number of length 10sentences :120</t>
+  </si>
+  <si>
+    <t>Number of length 11sentences :56</t>
+  </si>
+  <si>
+    <t>Number of length 12sentences :11</t>
+  </si>
+  <si>
+    <t>a 1672</t>
+  </si>
+  <si>
+    <t>is 472</t>
+  </si>
+  <si>
+    <t>man 413</t>
+  </si>
+  <si>
+    <t>in 335</t>
+  </si>
+  <si>
+    <t>of 304</t>
+  </si>
+  <si>
+    <t>are 290</t>
+  </si>
+  <si>
+    <t>the 267</t>
+  </si>
+  <si>
+    <t>Number of length 8sentences :34</t>
+  </si>
+  <si>
+    <t>Number of length 9sentences :225</t>
+  </si>
+  <si>
+    <t>Number of length 10sentences :160</t>
+  </si>
+  <si>
+    <t>Number of length 11sentences :548</t>
+  </si>
+  <si>
+    <t>Number of length 12sentences :27</t>
+  </si>
+  <si>
+    <t>a 2195</t>
+  </si>
+  <si>
+    <t>in 1016</t>
+  </si>
+  <si>
+    <t>is 716</t>
+  </si>
+  <si>
+    <t>shirt 546</t>
+  </si>
+  <si>
+    <t>man 537</t>
+  </si>
+  <si>
+    <t>of 481</t>
+  </si>
+  <si>
+    <t>the 370</t>
+  </si>
+  <si>
+    <t>RNN LDA Gauss</t>
+  </si>
+  <si>
+    <t>RNN img once + LDA</t>
+  </si>
+  <si>
+    <t>rnnlda_imgonce_struct.json</t>
   </si>
 </sst>
 </file>
@@ -348,7 +689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -358,59 +699,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <u/>
@@ -524,17 +822,6 @@
         <i val="0"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <u/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -546,6 +833,1155 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad2!$H$17:$H$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad2!$I$17:$I$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad2!$H$17:$H$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad2!$J$17:$J$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="383330592"/>
+        <c:axId val="383336576"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="383330592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="383336576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="383336576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="383330592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="206">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>347662</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>42862</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -811,10 +2247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P62"/>
+  <dimension ref="B1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,10 +2268,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
@@ -925,20 +2361,20 @@
       <c r="D4">
         <v>0.85</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <f>E3*$D$4</f>
         <v>55.165000000000006</v>
       </c>
-      <c r="F4" s="8">
-        <f t="shared" ref="F4:H4" si="0">F3*$D$4</f>
+      <c r="F4" s="7">
+        <f>F3*$D$4</f>
         <v>36.634999999999998</v>
       </c>
-      <c r="G4" s="8">
-        <f t="shared" si="0"/>
+      <c r="G4" s="7">
+        <f>G3*$D$4</f>
         <v>23.885000000000002</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f>H3*$D$4</f>
         <v>15.13</v>
       </c>
       <c r="O4" s="3" t="s">
@@ -1286,612 +2722,669 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>196</v>
+      </c>
       <c r="C13" t="s">
+        <v>195</v>
+      </c>
+      <c r="D13">
+        <v>24.58</v>
+      </c>
+      <c r="E13" s="9">
+        <v>63.2</v>
+      </c>
+      <c r="F13" s="9">
+        <v>41.7</v>
+      </c>
+      <c r="G13" s="9">
+        <v>27</v>
+      </c>
+      <c r="H13" s="9">
+        <v>17.2</v>
+      </c>
+      <c r="I13" s="9">
+        <v>15.2</v>
+      </c>
+      <c r="J13">
+        <v>228</v>
+      </c>
+      <c r="K13">
+        <v>7.875</v>
+      </c>
+      <c r="L13" s="9">
+        <v>743</v>
+      </c>
+      <c r="M13">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>59.8</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>39.1</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>25.1</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>16.100000000000001</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O14" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14">
-        <v>24.82</v>
-      </c>
-      <c r="E14">
-        <v>63.5</v>
-      </c>
-      <c r="F14">
-        <v>42.5</v>
-      </c>
-      <c r="G14">
-        <v>27.9</v>
-      </c>
-      <c r="H14">
-        <v>18</v>
-      </c>
-      <c r="I14">
-        <v>15.5</v>
-      </c>
-      <c r="J14">
-        <v>276</v>
-      </c>
-      <c r="K14">
-        <v>7.9930000000000003</v>
-      </c>
-      <c r="L14">
-        <v>786</v>
-      </c>
-      <c r="M14">
-        <v>461</v>
-      </c>
-      <c r="O14" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>24.82</v>
       </c>
       <c r="E15">
-        <v>62.1</v>
+        <v>63.5</v>
       </c>
       <c r="F15">
-        <v>41.6</v>
+        <v>42.5</v>
       </c>
       <c r="G15">
-        <v>27.6</v>
+        <v>27.9</v>
       </c>
       <c r="H15">
-        <v>18.2</v>
+        <v>18</v>
       </c>
       <c r="I15">
-        <v>16.77</v>
+        <v>15.5</v>
       </c>
       <c r="J15">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="K15">
-        <v>10.382999999999999</v>
-      </c>
-      <c r="L15" s="4">
-        <v>911</v>
+        <v>7.9930000000000003</v>
+      </c>
+      <c r="L15">
+        <v>786</v>
       </c>
       <c r="M15">
-        <v>482</v>
+        <v>461</v>
       </c>
       <c r="O15" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16">
         <v>24.82</v>
       </c>
       <c r="E16">
-        <v>60.4</v>
+        <v>62.1</v>
       </c>
       <c r="F16">
-        <v>40.4</v>
+        <v>41.6</v>
       </c>
       <c r="G16">
-        <v>26.8</v>
+        <v>27.6</v>
       </c>
       <c r="H16">
-        <v>17.600000000000001</v>
+        <v>18.2</v>
       </c>
       <c r="I16">
-        <v>15.5</v>
+        <v>16.77</v>
       </c>
       <c r="J16">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="K16">
-        <v>7.9770000000000003</v>
+        <v>10.382999999999999</v>
+      </c>
+      <c r="L16" s="4">
+        <v>911</v>
+      </c>
+      <c r="M16">
+        <v>482</v>
       </c>
       <c r="O16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17">
-        <v>23.62</v>
-      </c>
-      <c r="E17" s="4">
-        <v>63.7</v>
-      </c>
-      <c r="F17" s="4">
-        <v>43.4</v>
-      </c>
-      <c r="G17" s="4">
-        <v>29.2</v>
-      </c>
-      <c r="H17" s="4">
-        <v>19.3</v>
+        <v>24.82</v>
+      </c>
+      <c r="E17">
+        <v>60.4</v>
+      </c>
+      <c r="F17">
+        <v>40.4</v>
+      </c>
+      <c r="G17">
+        <v>26.8</v>
+      </c>
+      <c r="H17">
+        <v>17.600000000000001</v>
       </c>
       <c r="I17">
-        <v>15.76</v>
+        <v>15.5</v>
       </c>
       <c r="J17">
-        <v>347</v>
+        <v>277</v>
       </c>
       <c r="K17">
-        <v>7.96</v>
-      </c>
-      <c r="L17">
-        <v>775</v>
-      </c>
-      <c r="M17" s="4">
-        <v>557</v>
-      </c>
-      <c r="N17" t="s">
-        <v>50</v>
+        <v>7.9770000000000003</v>
       </c>
       <c r="O17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18">
         <v>23.62</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="4">
+        <v>63.7</v>
+      </c>
+      <c r="F18" s="4">
+        <v>43.4</v>
+      </c>
+      <c r="G18" s="4">
+        <v>29.2</v>
+      </c>
+      <c r="H18" s="4">
+        <v>19.3</v>
+      </c>
+      <c r="I18">
+        <v>15.76</v>
+      </c>
+      <c r="J18">
+        <v>347</v>
+      </c>
+      <c r="K18">
+        <v>7.96</v>
+      </c>
+      <c r="L18">
+        <v>775</v>
+      </c>
+      <c r="M18" s="4">
+        <v>557</v>
+      </c>
+      <c r="N18" t="s">
+        <v>50</v>
+      </c>
+      <c r="O18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19">
+        <v>23.62</v>
+      </c>
+      <c r="E19">
         <v>62.1</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>41.9</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>28.2</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <v>18.7</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I19" s="4">
         <v>17.18</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J19" s="4">
         <v>383</v>
       </c>
-      <c r="K18">
+      <c r="K19">
         <v>10.362</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L19" s="4">
         <v>915</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M19" s="4">
         <v>602</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N19" t="s">
         <v>53</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O19" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20">
-        <v>63.3</v>
-      </c>
-      <c r="F20">
-        <v>42.4</v>
-      </c>
-      <c r="G20">
-        <v>28.2</v>
-      </c>
-      <c r="H20">
-        <v>18.3</v>
-      </c>
-      <c r="I20">
-        <v>15.08</v>
-      </c>
-      <c r="J20">
-        <v>308</v>
-      </c>
-      <c r="K20">
-        <v>7.81</v>
-      </c>
-      <c r="L20">
-        <v>833</v>
-      </c>
-      <c r="M20">
-        <v>531</v>
-      </c>
-      <c r="O20" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21">
+        <v>63.3</v>
+      </c>
+      <c r="F21">
+        <v>42.4</v>
+      </c>
+      <c r="G21">
+        <v>28.2</v>
+      </c>
+      <c r="H21">
+        <v>18.3</v>
+      </c>
+      <c r="I21">
+        <v>15.08</v>
+      </c>
+      <c r="J21">
+        <v>308</v>
+      </c>
+      <c r="K21">
+        <v>7.81</v>
+      </c>
+      <c r="L21">
+        <v>833</v>
+      </c>
+      <c r="M21">
+        <v>531</v>
+      </c>
+      <c r="O21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>74</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>66</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>40.700000000000003</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>23.2</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>13.4</v>
       </c>
-      <c r="H21">
+      <c r="H22">
         <v>7.6</v>
       </c>
-      <c r="I21">
+      <c r="I22">
         <v>12.82</v>
       </c>
-      <c r="J21">
+      <c r="J22">
         <v>721</v>
       </c>
-      <c r="K21">
+      <c r="K22">
         <v>10.542999999999999</v>
       </c>
-      <c r="L21" s="6">
+      <c r="L22" s="6">
         <v>991</v>
       </c>
-      <c r="M21" s="6">
+      <c r="M22" s="6">
         <v>927</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+    <row r="23" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <v>66.3</v>
       </c>
-      <c r="F23">
+      <c r="F24">
         <v>42.3</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <v>27.7</v>
       </c>
-      <c r="H23">
+      <c r="H24">
         <v>18.3</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O24" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24">
-        <v>64.599999999999994</v>
-      </c>
-      <c r="F24">
-        <v>44.6</v>
-      </c>
-      <c r="G24">
-        <v>30.5</v>
-      </c>
-      <c r="H24">
-        <v>20.6</v>
-      </c>
-      <c r="I24">
-        <v>17.91</v>
-      </c>
-      <c r="O24" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25">
-        <v>59.8</v>
+        <v>64.599999999999994</v>
       </c>
       <c r="F25">
-        <v>41.3</v>
+        <v>44.6</v>
       </c>
       <c r="G25">
-        <v>29.3</v>
+        <v>30.5</v>
       </c>
       <c r="H25">
-        <v>19.2</v>
+        <v>20.6</v>
       </c>
       <c r="I25">
-        <v>18.579999999999998</v>
+        <v>17.91</v>
       </c>
       <c r="O25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E26">
-        <v>66.900000000000006</v>
+        <v>59.8</v>
       </c>
       <c r="F26">
-        <v>43.9</v>
+        <v>41.3</v>
       </c>
       <c r="G26">
-        <v>29.6</v>
+        <v>29.3</v>
       </c>
       <c r="H26">
-        <v>19.899999999999999</v>
+        <v>19.2</v>
       </c>
       <c r="I26">
-        <v>18.46</v>
+        <v>18.579999999999998</v>
       </c>
       <c r="O26" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="E27">
-        <v>57.3</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="F27">
-        <v>36.9</v>
+        <v>43.9</v>
       </c>
       <c r="G27">
-        <v>24</v>
+        <v>29.6</v>
       </c>
       <c r="H27">
-        <v>15.7</v>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="I27">
+        <v>18.46</v>
       </c>
       <c r="O27" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28">
+        <v>57.3</v>
+      </c>
+      <c r="F28">
+        <v>36.9</v>
+      </c>
+      <c r="G28">
+        <v>24</v>
+      </c>
+      <c r="H28">
+        <v>15.7</v>
+      </c>
+      <c r="O28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>26</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <v>67</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <v>47.5</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>33</v>
       </c>
-      <c r="H28">
+      <c r="H29">
         <v>24.3</v>
       </c>
-      <c r="I28">
+      <c r="I29">
         <v>19.399999999999999</v>
       </c>
-      <c r="O28" t="s">
+      <c r="O29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>67</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>68</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>29.7</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>43.7</v>
       </c>
-      <c r="F31">
+      <c r="F32">
         <v>25.5</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>14.6</v>
       </c>
-      <c r="H31">
+      <c r="H32">
         <v>9</v>
       </c>
-      <c r="I31">
+      <c r="I32">
         <v>12.52</v>
       </c>
-      <c r="J31">
+      <c r="J32">
         <v>248</v>
       </c>
-      <c r="K31">
+      <c r="K32">
         <v>13.862</v>
       </c>
-      <c r="L31">
+      <c r="L32">
         <v>993</v>
       </c>
-      <c r="M31">
+      <c r="M32">
         <v>738</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N32" t="s">
         <v>78</v>
       </c>
-      <c r="O31" t="s">
+      <c r="O32" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32">
-        <v>29.75</v>
-      </c>
-      <c r="O32" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D33">
-        <v>29.27</v>
+        <v>29.75</v>
       </c>
       <c r="E33">
-        <v>57.4</v>
+        <v>55.3</v>
       </c>
       <c r="F33">
-        <v>36.200000000000003</v>
+        <v>33.6</v>
       </c>
       <c r="G33">
-        <v>22.6</v>
+        <v>20.2</v>
       </c>
       <c r="H33">
-        <v>14.3</v>
+        <v>12.7</v>
       </c>
       <c r="I33">
-        <v>13.53</v>
+        <v>12.7</v>
       </c>
       <c r="J33">
-        <v>179</v>
+        <v>208</v>
       </c>
       <c r="K33">
-        <v>8.9540000000000006</v>
+        <v>9.5960000000000001</v>
       </c>
       <c r="L33">
-        <v>844</v>
+        <v>912</v>
       </c>
       <c r="M33">
-        <v>420</v>
+        <v>363</v>
       </c>
       <c r="N33" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="O33" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34">
+        <v>29.75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35">
+        <v>29.27</v>
+      </c>
+      <c r="E35">
+        <v>57.4</v>
+      </c>
+      <c r="F35">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="G35">
+        <v>22.6</v>
+      </c>
+      <c r="H35">
+        <v>14.3</v>
+      </c>
+      <c r="I35">
+        <v>13.53</v>
+      </c>
+      <c r="J35">
+        <v>179</v>
+      </c>
+      <c r="K35">
+        <v>8.9540000000000006</v>
+      </c>
+      <c r="L35">
+        <v>844</v>
+      </c>
+      <c r="M35">
+        <v>420</v>
+      </c>
+      <c r="N35" t="s">
+        <v>78</v>
+      </c>
+      <c r="O35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>79</v>
       </c>
-      <c r="O34" t="s">
+      <c r="O36" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>32</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>34</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D40" t="s">
         <v>33</v>
       </c>
-      <c r="J38">
+      <c r="J40">
         <v>19.7</v>
-      </c>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" t="s">
-        <v>39</v>
-      </c>
-      <c r="J39">
-        <v>19.8</v>
-      </c>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" t="s">
-        <v>48</v>
-      </c>
-      <c r="J40">
-        <v>19.8</v>
       </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="J41">
-        <v>20.2</v>
+        <v>19.8</v>
       </c>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="D42" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="J42">
         <v>19.8</v>
@@ -1899,270 +3392,252 @@
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" t="s">
+        <v>61</v>
+      </c>
+      <c r="J43">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" t="s">
+        <v>72</v>
+      </c>
+      <c r="J44">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
         <v>82</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D45" t="s">
         <v>83</v>
       </c>
-      <c r="J43">
+      <c r="J45">
         <v>14.2</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" t="s">
+        <v>88</v>
+      </c>
+      <c r="J46">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>71</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C49" t="s">
         <v>70</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D49" s="3">
         <v>23.16</v>
-      </c>
-    </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>57.9</v>
-      </c>
-      <c r="F47">
-        <v>39.1</v>
-      </c>
-      <c r="G47">
-        <v>25.5</v>
-      </c>
-      <c r="H47">
-        <v>16.3</v>
-      </c>
-    </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48">
-        <v>5</v>
-      </c>
-      <c r="E48">
-        <v>62.6</v>
-      </c>
-      <c r="F48">
-        <v>42.6</v>
-      </c>
-      <c r="G48">
-        <v>28.3</v>
-      </c>
-      <c r="H48">
-        <v>18.600000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49">
-        <v>10</v>
-      </c>
-      <c r="E49">
-        <v>63.6</v>
-      </c>
-      <c r="F49">
-        <v>42.9</v>
-      </c>
-      <c r="G49">
-        <v>28.4</v>
-      </c>
-      <c r="H49">
-        <v>18.5</v>
       </c>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E50">
-        <v>64.400000000000006</v>
+        <v>57.9</v>
       </c>
       <c r="F50">
-        <v>43.3</v>
+        <v>39.1</v>
       </c>
       <c r="G50">
-        <v>28.4</v>
+        <v>25.5</v>
       </c>
       <c r="H50">
-        <v>18.399999999999999</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E51">
-        <v>64.400000000000006</v>
+        <v>62.6</v>
       </c>
       <c r="F51">
-        <v>43.2</v>
+        <v>42.6</v>
       </c>
       <c r="G51">
-        <v>28.1</v>
+        <v>28.3</v>
       </c>
       <c r="H51">
-        <v>17.8</v>
-      </c>
-      <c r="I51">
-        <v>15.95</v>
-      </c>
-      <c r="J51">
-        <v>296</v>
-      </c>
-      <c r="K51">
-        <v>8.3249999999999993</v>
-      </c>
-      <c r="L51">
-        <v>775</v>
-      </c>
-      <c r="M51">
-        <v>490</v>
+        <v>18.600000000000001</v>
       </c>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="E52">
-        <v>64.900000000000006</v>
+        <v>63.6</v>
       </c>
       <c r="F52">
-        <v>43.7</v>
+        <v>42.9</v>
       </c>
       <c r="G52">
-        <v>28.5</v>
+        <v>28.4</v>
       </c>
       <c r="H52">
-        <v>18.2</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="E53">
-        <v>64.7</v>
+        <v>64.400000000000006</v>
       </c>
       <c r="F53">
-        <v>43.4</v>
+        <v>43.3</v>
       </c>
       <c r="G53">
-        <v>28.2</v>
+        <v>28.4</v>
       </c>
       <c r="H53">
-        <v>17.899999999999999</v>
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>50</v>
+      </c>
+      <c r="E54">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="F54">
+        <v>43.2</v>
+      </c>
+      <c r="G54">
+        <v>28.1</v>
+      </c>
+      <c r="H54">
+        <v>17.8</v>
+      </c>
+      <c r="I54">
+        <v>15.95</v>
+      </c>
+      <c r="J54">
+        <v>296</v>
+      </c>
+      <c r="K54">
+        <v>8.3249999999999993</v>
+      </c>
+      <c r="L54">
+        <v>775</v>
+      </c>
+      <c r="M54">
+        <v>490</v>
       </c>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>57</v>
-      </c>
-      <c r="D55" s="3">
-        <v>23.16</v>
+      <c r="B55">
+        <v>75</v>
+      </c>
+      <c r="E55">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="F55">
+        <v>43.7</v>
+      </c>
+      <c r="G55">
+        <v>28.5</v>
+      </c>
+      <c r="H55">
+        <v>18.2</v>
       </c>
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E56">
-        <v>57.9</v>
+        <v>64.7</v>
       </c>
       <c r="F56">
-        <v>39.1</v>
+        <v>43.4</v>
       </c>
       <c r="G56">
-        <v>25.5</v>
+        <v>28.2</v>
       </c>
       <c r="H56">
-        <v>16.3</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B57">
-        <v>5</v>
-      </c>
-      <c r="E57">
-        <v>62.1</v>
-      </c>
-      <c r="F57">
-        <v>42.4</v>
-      </c>
-      <c r="G57">
-        <v>28.6</v>
-      </c>
-      <c r="H57">
-        <v>19.100000000000001</v>
+        <v>17.899999999999999</v>
       </c>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B58">
-        <v>10</v>
-      </c>
-      <c r="E58">
-        <v>62.9</v>
-      </c>
-      <c r="F58">
-        <v>42.8</v>
-      </c>
-      <c r="G58">
-        <v>28.8</v>
-      </c>
-      <c r="H58">
-        <v>19.2</v>
+      <c r="C58" t="s">
+        <v>57</v>
+      </c>
+      <c r="D58" s="3">
+        <v>23.16</v>
       </c>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B59">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E59">
-        <v>62.9</v>
+        <v>57.9</v>
       </c>
       <c r="F59">
-        <v>42.7</v>
+        <v>39.1</v>
       </c>
       <c r="G59">
-        <v>28.9</v>
+        <v>25.5</v>
       </c>
       <c r="H59">
-        <v>19.399999999999999</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B60">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E60">
-        <v>62.7</v>
+        <v>62.1</v>
       </c>
       <c r="F60">
-        <v>42.5</v>
+        <v>42.4</v>
       </c>
       <c r="G60">
-        <v>28.8</v>
+        <v>28.6</v>
       </c>
       <c r="H60">
-        <v>19.399999999999999</v>
+        <v>19.100000000000001</v>
       </c>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B61">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="E61">
-        <v>62.5</v>
+        <v>62.9</v>
       </c>
       <c r="F61">
-        <v>42.2</v>
+        <v>42.8</v>
       </c>
       <c r="G61">
-        <v>28.5</v>
+        <v>28.8</v>
       </c>
       <c r="H61">
         <v>19.2</v>
@@ -2170,6 +3645,57 @@
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B62">
+        <v>25</v>
+      </c>
+      <c r="E62">
+        <v>62.9</v>
+      </c>
+      <c r="F62">
+        <v>42.7</v>
+      </c>
+      <c r="G62">
+        <v>28.9</v>
+      </c>
+      <c r="H62">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>50</v>
+      </c>
+      <c r="E63">
+        <v>62.7</v>
+      </c>
+      <c r="F63">
+        <v>42.5</v>
+      </c>
+      <c r="G63">
+        <v>28.8</v>
+      </c>
+      <c r="H63">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>75</v>
+      </c>
+      <c r="E64">
+        <v>62.5</v>
+      </c>
+      <c r="F64">
+        <v>42.2</v>
+      </c>
+      <c r="G64">
+        <v>28.5</v>
+      </c>
+      <c r="H64">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65">
         <v>100</v>
       </c>
     </row>
@@ -2177,67 +3703,708 @@
   <mergeCells count="1">
     <mergeCell ref="E1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="K14:K16 E3:E29 E31 F4:H4">
-    <cfRule type="top10" dxfId="27" priority="30" rank="1"/>
+  <conditionalFormatting sqref="K15:K17 E3:E30 F4:H4 E32:E34">
+    <cfRule type="top10" dxfId="19" priority="30" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31 F3 F5:F29">
-    <cfRule type="top10" dxfId="26" priority="34" rank="1"/>
+  <conditionalFormatting sqref="F3 F5:F30 F32:F34">
+    <cfRule type="top10" dxfId="18" priority="34" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G31 G3 G5:G29">
-    <cfRule type="top10" dxfId="25" priority="37" rank="1"/>
+  <conditionalFormatting sqref="G3 G5:G30 G32:G34">
+    <cfRule type="top10" dxfId="17" priority="37" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31 H3 H5:H29">
-    <cfRule type="top10" dxfId="24" priority="40" rank="1"/>
+  <conditionalFormatting sqref="H3 H5:H30 H32:H34">
+    <cfRule type="top10" dxfId="16" priority="40" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E47:E53">
-    <cfRule type="top10" dxfId="23" priority="8" rank="1"/>
+  <conditionalFormatting sqref="E50:E56">
+    <cfRule type="top10" dxfId="15" priority="8" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F47:F53">
-    <cfRule type="top10" dxfId="22" priority="7" rank="1"/>
+  <conditionalFormatting sqref="F50:F56">
+    <cfRule type="top10" dxfId="14" priority="7" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G47:G53">
-    <cfRule type="top10" dxfId="21" priority="6" rank="1"/>
+  <conditionalFormatting sqref="G50:G56">
+    <cfRule type="top10" dxfId="13" priority="6" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47:H53">
-    <cfRule type="top10" dxfId="20" priority="5" rank="1"/>
+  <conditionalFormatting sqref="H50:H56">
+    <cfRule type="top10" dxfId="12" priority="5" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E56:E62">
-    <cfRule type="top10" dxfId="19" priority="4" rank="1"/>
+  <conditionalFormatting sqref="E59:E65">
+    <cfRule type="top10" dxfId="11" priority="4" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F56:F62">
-    <cfRule type="top10" dxfId="18" priority="3" rank="1"/>
+  <conditionalFormatting sqref="F59:F65">
+    <cfRule type="top10" dxfId="10" priority="3" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G56:G62">
-    <cfRule type="top10" dxfId="17" priority="2" rank="1"/>
+  <conditionalFormatting sqref="G59:G65">
+    <cfRule type="top10" dxfId="9" priority="2" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H56:H62">
-    <cfRule type="top10" dxfId="16" priority="1" rank="1"/>
+  <conditionalFormatting sqref="H59:H65">
+    <cfRule type="top10" dxfId="8" priority="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I28">
-    <cfRule type="top10" dxfId="15" priority="41" rank="1"/>
+  <conditionalFormatting sqref="I3:I29">
+    <cfRule type="top10" dxfId="7" priority="41" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E21 F4:H4">
-    <cfRule type="top10" dxfId="14" priority="52" rank="1"/>
+  <conditionalFormatting sqref="E3:E22 F4:H4">
+    <cfRule type="top10" dxfId="6" priority="52" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3 F5:F21">
-    <cfRule type="top10" dxfId="13" priority="54" rank="1"/>
+  <conditionalFormatting sqref="F3 F5:F22">
+    <cfRule type="top10" dxfId="5" priority="54" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3 G5:G21">
-    <cfRule type="top10" dxfId="12" priority="56" rank="1"/>
+  <conditionalFormatting sqref="G3 G5:G22">
+    <cfRule type="top10" dxfId="4" priority="56" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3 H5:H21">
-    <cfRule type="top10" dxfId="11" priority="58" rank="1"/>
+  <conditionalFormatting sqref="H3 H5:H22">
+    <cfRule type="top10" dxfId="3" priority="58" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I21">
-    <cfRule type="top10" dxfId="10" priority="60" rank="1"/>
+  <conditionalFormatting sqref="I3:I22">
+    <cfRule type="top10" dxfId="2" priority="60" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J21">
-    <cfRule type="top10" dxfId="9" priority="62" rank="1"/>
+  <conditionalFormatting sqref="J3:J22">
+    <cfRule type="top10" dxfId="1" priority="62" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K21">
-    <cfRule type="top10" dxfId="8" priority="64" rank="1"/>
+  <conditionalFormatting sqref="K3:K22">
+    <cfRule type="top10" dxfId="0" priority="64" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" t="s">
+        <v>166</v>
+      </c>
+      <c r="H4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G6" t="s">
+        <v>168</v>
+      </c>
+      <c r="H6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" t="s">
+        <v>144</v>
+      </c>
+      <c r="G7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" t="s">
+        <v>171</v>
+      </c>
+      <c r="H9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>97</v>
+      </c>
+      <c r="G11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>11</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" t="s">
+        <v>135</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" t="s">
+        <v>136</v>
+      </c>
+      <c r="E19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" t="s">
+        <v>136</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>27</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F20" t="s">
+        <v>137</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>96</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" t="s">
+        <v>138</v>
+      </c>
+      <c r="H21">
+        <v>6</v>
+      </c>
+      <c r="I21">
+        <v>228</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
+        <v>139</v>
+      </c>
+      <c r="E22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" t="s">
+        <v>139</v>
+      </c>
+      <c r="H22">
+        <v>7</v>
+      </c>
+      <c r="I22">
+        <v>328</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23">
+        <v>8</v>
+      </c>
+      <c r="I23">
+        <v>102</v>
+      </c>
+      <c r="J23">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" t="s">
+        <v>110</v>
+      </c>
+      <c r="H24">
+        <v>9</v>
+      </c>
+      <c r="I24">
+        <v>93</v>
+      </c>
+      <c r="J24">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" t="s">
+        <v>124</v>
+      </c>
+      <c r="H25">
+        <v>10</v>
+      </c>
+      <c r="I25">
+        <v>26</v>
+      </c>
+      <c r="J25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26">
+        <v>11</v>
+      </c>
+      <c r="I26">
+        <v>61</v>
+      </c>
+      <c r="J26">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="H27">
+        <v>12</v>
+      </c>
+      <c r="I27">
+        <v>19</v>
+      </c>
+      <c r="J27">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>123</v>
+      </c>
+      <c r="H28">
+        <v>13</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+      <c r="H29">
+        <v>14</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+      <c r="H30">
+        <v>15</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>125</v>
+      </c>
+      <c r="H31">
+        <v>20</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E34" t="s">
+        <v>103</v>
+      </c>
+      <c r="F34" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" t="s">
+        <v>182</v>
+      </c>
+      <c r="F35" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" t="s">
+        <v>160</v>
+      </c>
+      <c r="E36" t="s">
+        <v>183</v>
+      </c>
+      <c r="F36" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" t="s">
+        <v>161</v>
+      </c>
+      <c r="E37" t="s">
+        <v>184</v>
+      </c>
+      <c r="F37" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" t="s">
+        <v>162</v>
+      </c>
+      <c r="E38" t="s">
+        <v>185</v>
+      </c>
+      <c r="F38" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>152</v>
+      </c>
+      <c r="C39" t="s">
+        <v>163</v>
+      </c>
+      <c r="E39" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" t="s">
+        <v>164</v>
+      </c>
+      <c r="E40" t="s">
+        <v>99</v>
+      </c>
+      <c r="F40" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>154</v>
+      </c>
+      <c r="E41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>